<commit_message>
EMC: - dalsi slajdy
</commit_message>
<xml_diff>
--- a/EMC/Data/model vedeni.xlsx
+++ b/EMC/Data/model vedeni.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -10,7 +10,7 @@
     <sheet name="List1" sheetId="1" r:id="rId1"/>
     <sheet name="Antena" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -170,7 +170,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv systému Office">
   <a:themeElements>
     <a:clrScheme name="Kancelář">
       <a:dk1>
@@ -212,7 +212,7 @@
     </a:clrScheme>
     <a:fontScheme name="Kancelář">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -247,7 +247,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -575,10 +575,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B9"/>
+  <dimension ref="A2:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,7 +586,7 @@
     <col min="2" max="2" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -594,8 +594,11 @@
         <f>0.125</f>
         <v>0.125</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -603,8 +606,11 @@
         <f>B2/4</f>
         <v>3.125E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D3" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -612,8 +618,12 @@
         <f>B3</f>
         <v>3.125E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D4" s="1">
+        <f>D3/(D2^2)</f>
+        <v>3.9999999999999996E-10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -622,7 +632,7 @@
         <v>0.15309310892394862</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -631,10 +641,10 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
     </row>
   </sheetData>

</xml_diff>